<commit_message>
checked the 2 Excel mappings files, and removed references to previous versions of RiC-O
</commit_message>
<xml_diff>
--- a/docs/EAC_to_RiC-O_1.1_documentation.xlsx
+++ b/docs/EAC_to_RiC-O_1.1_documentation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\shared\ArchivesNationalesFr\rico-converter\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7D91481-A565-4F90-BBA5-C216104E2502}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4EE697F-D09E-46D3-AB7E-37CDDC40D1F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33795" yWindow="1890" windowWidth="21600" windowHeight="11235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuille 1" sheetId="1" r:id="rId1"/>
@@ -35,9 +35,6 @@
   </si>
   <si>
     <t>EAC-CPF XPath</t>
-  </si>
-  <si>
-    <t>RiC-O 1.0 Classes and Properties involved</t>
   </si>
   <si>
     <t>Notes</t>
@@ -2377,6 +2374,9 @@
       </rPr>
       <t xml:space="preserve"> on the relation</t>
     </r>
+  </si>
+  <si>
+    <t>RiC-O 1.1 Classes and Properties involved</t>
   </si>
 </sst>
 </file>
@@ -2482,7 +2482,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -2529,17 +2529,11 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2773,7 +2767,7 @@
   </sheetPr>
   <dimension ref="A1:AA994"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
       <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
@@ -2791,15 +2785,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
-        <v>256</v>
-      </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
+      <c r="A1" s="19" t="s">
+        <v>255</v>
+      </c>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
       <c r="H1" s="3"/>
       <c r="I1" s="2"/>
     </row>
@@ -2820,35 +2814,35 @@
         <v>4</v>
       </c>
       <c r="F2" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="G2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="H2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="I2" s="6" t="s">
         <v>7</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:27" ht="224.4" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3" s="8"/>
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
       <c r="E3" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="8" t="s">
         <v>10</v>
-      </c>
-      <c r="F3" s="19" t="s">
-        <v>11</v>
       </c>
       <c r="G3" s="8"/>
       <c r="H3" s="9"/>
       <c r="I3" s="9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J3" s="10"/>
       <c r="K3" s="10"/>
@@ -2871,25 +2865,25 @@
     </row>
     <row r="4" spans="1:27" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C4" s="8"/>
       <c r="D4" s="8"/>
       <c r="E4" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="8" t="s">
         <v>14</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>15</v>
       </c>
       <c r="G4" s="8"/>
       <c r="H4" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I4" s="9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J4" s="10"/>
       <c r="K4" s="10"/>
@@ -2912,25 +2906,25 @@
     </row>
     <row r="5" spans="1:27" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C5" s="8"/>
       <c r="D5" s="8"/>
       <c r="E5" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="8" t="s">
         <v>18</v>
-      </c>
-      <c r="F5" s="8" t="s">
-        <v>19</v>
       </c>
       <c r="G5" s="8"/>
       <c r="H5" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="I5" s="9" t="s">
         <v>20</v>
-      </c>
-      <c r="I5" s="9" t="s">
-        <v>21</v>
       </c>
       <c r="J5" s="10"/>
       <c r="K5" s="10"/>
@@ -2953,22 +2947,22 @@
     </row>
     <row r="6" spans="1:27" ht="66" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C6" s="8"/>
       <c r="D6" s="8"/>
       <c r="E6" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" s="11" t="s">
         <v>23</v>
-      </c>
-      <c r="F6" s="11" t="s">
-        <v>24</v>
       </c>
       <c r="G6" s="11"/>
       <c r="H6" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I6" s="9"/>
       <c r="J6" s="10"/>
@@ -2992,22 +2986,22 @@
     </row>
     <row r="7" spans="1:27" ht="66" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C7" s="8"/>
       <c r="D7" s="8"/>
       <c r="E7" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G7" s="11"/>
       <c r="H7" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I7" s="9"/>
       <c r="J7" s="10"/>
@@ -3031,25 +3025,25 @@
     </row>
     <row r="8" spans="1:27" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C8" s="8"/>
       <c r="D8" s="8"/>
       <c r="E8" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="F8" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="G8" s="19" t="s">
-        <v>253</v>
+      <c r="G8" s="8" t="s">
+        <v>252</v>
       </c>
       <c r="H8" s="9"/>
       <c r="I8" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J8" s="10"/>
       <c r="K8" s="10"/>
@@ -3072,25 +3066,25 @@
     </row>
     <row r="9" spans="1:27" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C9" s="8"/>
       <c r="D9" s="8"/>
       <c r="E9" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="F9" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="F9" s="9" t="s">
+      <c r="G9" s="9" t="s">
         <v>34</v>
-      </c>
-      <c r="G9" s="9" t="s">
-        <v>35</v>
       </c>
       <c r="H9" s="9"/>
       <c r="I9" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J9" s="13"/>
       <c r="K9" s="13"/>
@@ -3113,25 +3107,25 @@
     </row>
     <row r="10" spans="1:27" ht="105.6" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C10" s="8"/>
       <c r="D10" s="8"/>
       <c r="E10" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="F10" s="8" t="s">
         <v>38</v>
-      </c>
-      <c r="F10" s="8" t="s">
-        <v>39</v>
       </c>
       <c r="G10" s="8"/>
       <c r="H10" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="I10" s="9" t="s">
         <v>40</v>
-      </c>
-      <c r="I10" s="9" t="s">
-        <v>41</v>
       </c>
       <c r="J10" s="13"/>
       <c r="K10" s="13"/>
@@ -3154,18 +3148,18 @@
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C11" s="8"/>
       <c r="D11" s="8"/>
       <c r="E11" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F11" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G11" s="11"/>
       <c r="H11" s="9"/>
@@ -3191,18 +3185,18 @@
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C12" s="8"/>
       <c r="D12" s="8"/>
       <c r="E12" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F12" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G12" s="11"/>
       <c r="H12" s="9"/>
@@ -3228,25 +3222,25 @@
     </row>
     <row r="13" spans="1:27" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B13" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" s="8" t="s">
         <v>46</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>47</v>
       </c>
       <c r="D13" s="8"/>
       <c r="E13" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="F13" s="8" t="s">
         <v>48</v>
-      </c>
-      <c r="F13" s="8" t="s">
-        <v>49</v>
       </c>
       <c r="G13" s="8"/>
       <c r="H13" s="9"/>
       <c r="I13" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J13" s="10"/>
       <c r="K13" s="10"/>
@@ -3269,27 +3263,27 @@
     </row>
     <row r="14" spans="1:27" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B14" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C14" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="D14" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="D14" s="8" t="s">
+      <c r="E14" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="E14" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="F14" s="20" t="s">
-        <v>257</v>
+      <c r="F14" s="18" t="s">
+        <v>256</v>
       </c>
       <c r="G14" s="8"/>
       <c r="H14" s="9"/>
       <c r="I14" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J14" s="10"/>
       <c r="K14" s="10"/>
@@ -3312,29 +3306,29 @@
     </row>
     <row r="15" spans="1:27" ht="66" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B15" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C15" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="C15" s="8" t="s">
-        <v>52</v>
-      </c>
       <c r="D15" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="E15" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="E15" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="F15" s="19" t="s">
-        <v>258</v>
+      <c r="F15" s="8" t="s">
+        <v>257</v>
       </c>
       <c r="G15" s="8"/>
       <c r="H15" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="I15" s="9" t="s">
         <v>58</v>
-      </c>
-      <c r="I15" s="9" t="s">
-        <v>59</v>
       </c>
       <c r="J15" s="10"/>
       <c r="K15" s="10"/>
@@ -3357,27 +3351,27 @@
     </row>
     <row r="16" spans="1:27" ht="299.39999999999998" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B16" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="C16" s="8" t="s">
         <v>61</v>
-      </c>
-      <c r="C16" s="8" t="s">
-        <v>62</v>
       </c>
       <c r="D16" s="8"/>
       <c r="E16" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="F16" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="F16" s="8" t="s">
+      <c r="G16" s="9" t="s">
         <v>64</v>
-      </c>
-      <c r="G16" s="9" t="s">
-        <v>65</v>
       </c>
       <c r="H16" s="9"/>
       <c r="I16" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J16" s="10"/>
       <c r="K16" s="10"/>
@@ -3400,25 +3394,25 @@
     </row>
     <row r="17" spans="1:27" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B17" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="B17" s="8" t="s">
-        <v>61</v>
-      </c>
       <c r="C17" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D17" s="8"/>
       <c r="E17" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="F17" s="8" t="s">
         <v>68</v>
-      </c>
-      <c r="F17" s="8" t="s">
-        <v>69</v>
       </c>
       <c r="G17" s="8"/>
       <c r="H17" s="9"/>
       <c r="I17" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J17" s="10"/>
       <c r="K17" s="10"/>
@@ -3441,27 +3435,27 @@
     </row>
     <row r="18" spans="1:27" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B18" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="B18" s="8" t="s">
-        <v>61</v>
-      </c>
       <c r="C18" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D18" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="D18" s="8" t="s">
+      <c r="E18" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="E18" s="14" t="s">
-        <v>73</v>
-      </c>
-      <c r="F18" s="19" t="s">
-        <v>255</v>
+      <c r="F18" s="8" t="s">
+        <v>254</v>
       </c>
       <c r="G18" s="8"/>
       <c r="H18" s="9"/>
       <c r="I18" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J18" s="13"/>
       <c r="K18" s="13"/>
@@ -3484,21 +3478,21 @@
     </row>
     <row r="19" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B19" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="B19" s="8" t="s">
-        <v>61</v>
-      </c>
       <c r="C19" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D19" s="8"/>
       <c r="E19" s="11"/>
       <c r="F19" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G19" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I19" s="9"/>
       <c r="J19" s="10"/>
@@ -3522,29 +3516,29 @@
     </row>
     <row r="20" spans="1:27" ht="237.6" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B20" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="B20" s="8" t="s">
-        <v>61</v>
-      </c>
       <c r="C20" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D20" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="E20" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="E20" s="7" t="s">
+      <c r="F20" s="8" t="s">
         <v>78</v>
-      </c>
-      <c r="F20" s="8" t="s">
-        <v>79</v>
       </c>
       <c r="G20" s="8"/>
       <c r="H20" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I20" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J20" s="10"/>
       <c r="K20" s="10"/>
@@ -3567,29 +3561,29 @@
     </row>
     <row r="21" spans="1:27" ht="145.19999999999999" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B21" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="B21" s="8" t="s">
-        <v>61</v>
-      </c>
       <c r="C21" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D21" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="E21" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="E21" s="7" t="s">
+      <c r="F21" s="8" t="s">
         <v>82</v>
-      </c>
-      <c r="F21" s="8" t="s">
-        <v>83</v>
       </c>
       <c r="G21" s="8"/>
       <c r="H21" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I21" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J21" s="10"/>
       <c r="K21" s="10"/>
@@ -3612,29 +3606,29 @@
     </row>
     <row r="22" spans="1:27" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B22" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="B22" s="8" t="s">
-        <v>61</v>
-      </c>
       <c r="C22" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D22" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="E22" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="E22" s="7" t="s">
+      <c r="F22" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="F22" s="8" t="s">
+      <c r="G22" s="9" t="s">
         <v>87</v>
-      </c>
-      <c r="G22" s="9" t="s">
-        <v>88</v>
       </c>
       <c r="H22" s="9"/>
       <c r="I22" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J22" s="10"/>
       <c r="K22" s="10"/>
@@ -3657,22 +3651,22 @@
     </row>
     <row r="23" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B23" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="B23" s="8" t="s">
-        <v>61</v>
-      </c>
       <c r="C23" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D23" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="E23" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="E23" s="12" t="s">
-        <v>90</v>
-      </c>
       <c r="F23" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G23" s="11"/>
       <c r="H23" s="9"/>
@@ -3698,20 +3692,20 @@
     </row>
     <row r="24" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B24" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="B24" s="8" t="s">
-        <v>61</v>
-      </c>
       <c r="C24" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D24" s="8"/>
       <c r="E24" s="12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F24" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G24" s="11"/>
       <c r="H24" s="9"/>
@@ -3737,29 +3731,29 @@
     </row>
     <row r="25" spans="1:27" ht="105.6" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B25" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="C25" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="C25" s="8" t="s">
+      <c r="D25" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="D25" s="8" t="s">
+      <c r="E25" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="E25" s="8" t="s">
+      <c r="F25" s="8" t="s">
         <v>96</v>
-      </c>
-      <c r="F25" s="8" t="s">
-        <v>97</v>
       </c>
       <c r="G25" s="8"/>
       <c r="H25" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="I25" s="8" t="s">
         <v>98</v>
-      </c>
-      <c r="I25" s="8" t="s">
-        <v>99</v>
       </c>
       <c r="J25" s="15"/>
       <c r="K25" s="15"/>
@@ -3782,29 +3776,29 @@
     </row>
     <row r="26" spans="1:27" ht="132" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C26" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="D26" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="D26" s="8" t="s">
+      <c r="E26" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="E26" s="8" t="s">
+      <c r="F26" s="8" t="s">
         <v>102</v>
-      </c>
-      <c r="F26" s="19" t="s">
-        <v>103</v>
       </c>
       <c r="G26" s="8"/>
       <c r="H26" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="I26" s="9" t="s">
         <v>104</v>
-      </c>
-      <c r="I26" s="9" t="s">
-        <v>105</v>
       </c>
       <c r="J26" s="10"/>
       <c r="K26" s="10"/>
@@ -3827,29 +3821,29 @@
     </row>
     <row r="27" spans="1:27" ht="184.8" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D27" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="E27" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="E27" s="8" t="s">
+      <c r="F27" s="8" t="s">
         <v>107</v>
-      </c>
-      <c r="F27" s="19" t="s">
-        <v>108</v>
       </c>
       <c r="G27" s="8"/>
       <c r="H27" s="9" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I27" s="9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J27" s="10"/>
       <c r="K27" s="10"/>
@@ -3872,29 +3866,29 @@
     </row>
     <row r="28" spans="1:27" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D28" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="E28" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="E28" s="12" t="s">
+      <c r="F28" s="8" t="s">
+        <v>248</v>
+      </c>
+      <c r="G28" s="8" t="s">
         <v>111</v>
-      </c>
-      <c r="F28" s="8" t="s">
-        <v>249</v>
-      </c>
-      <c r="G28" s="8" t="s">
-        <v>112</v>
       </c>
       <c r="H28" s="9"/>
       <c r="I28" s="9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J28" s="10"/>
       <c r="K28" s="10"/>
@@ -3917,27 +3911,27 @@
     </row>
     <row r="29" spans="1:27" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D29" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="E29" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="E29" s="8" t="s">
+      <c r="F29" s="8" t="s">
         <v>115</v>
-      </c>
-      <c r="F29" s="8" t="s">
-        <v>116</v>
       </c>
       <c r="G29" s="8"/>
       <c r="H29" s="9"/>
       <c r="I29" s="9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J29" s="10"/>
       <c r="K29" s="10"/>
@@ -3960,26 +3954,26 @@
     </row>
     <row r="30" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D30" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="E30" s="12" t="s">
         <v>117</v>
       </c>
-      <c r="E30" s="12" t="s">
+      <c r="F30" s="11" t="s">
         <v>118</v>
-      </c>
-      <c r="F30" s="11" t="s">
-        <v>119</v>
       </c>
       <c r="G30" s="11"/>
       <c r="H30" s="9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I30" s="9"/>
       <c r="J30" s="10"/>
@@ -4003,27 +3997,27 @@
     </row>
     <row r="31" spans="1:27" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D31" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="E31" s="12" t="s">
         <v>121</v>
       </c>
-      <c r="E31" s="12" t="s">
-        <v>122</v>
-      </c>
-      <c r="F31" s="19" t="s">
-        <v>259</v>
+      <c r="F31" s="8" t="s">
+        <v>258</v>
       </c>
       <c r="G31" s="8"/>
       <c r="H31" s="9"/>
       <c r="I31" s="9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J31" s="10"/>
       <c r="K31" s="10"/>
@@ -4046,26 +4040,26 @@
     </row>
     <row r="32" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D32" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="E32" s="12" t="s">
         <v>123</v>
       </c>
-      <c r="E32" s="12" t="s">
-        <v>124</v>
-      </c>
       <c r="F32" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G32" s="8"/>
       <c r="H32" s="9" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I32" s="9"/>
       <c r="J32" s="10"/>
@@ -4089,29 +4083,29 @@
     </row>
     <row r="33" spans="1:27" ht="158.4" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C33" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="D33" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="D33" s="8" t="s">
+      <c r="E33" s="8" t="s">
         <v>127</v>
       </c>
-      <c r="E33" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="F33" s="19" t="s">
-        <v>243</v>
+      <c r="F33" s="8" t="s">
+        <v>242</v>
       </c>
       <c r="G33" s="8"/>
       <c r="H33" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="I33" s="9" t="s">
         <v>129</v>
-      </c>
-      <c r="I33" s="9" t="s">
-        <v>130</v>
       </c>
       <c r="J33" s="10"/>
       <c r="K33" s="10"/>
@@ -4134,29 +4128,29 @@
     </row>
     <row r="34" spans="1:27" ht="211.2" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C34" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="D34" s="8" t="s">
         <v>131</v>
       </c>
-      <c r="D34" s="8" t="s">
+      <c r="E34" s="8" t="s">
         <v>132</v>
       </c>
-      <c r="E34" s="8" t="s">
+      <c r="F34" s="9" t="s">
         <v>133</v>
-      </c>
-      <c r="F34" s="21" t="s">
-        <v>134</v>
       </c>
       <c r="G34" s="9"/>
       <c r="H34" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="I34" s="9" t="s">
         <v>135</v>
-      </c>
-      <c r="I34" s="9" t="s">
-        <v>136</v>
       </c>
       <c r="J34" s="10"/>
       <c r="K34" s="10"/>
@@ -4179,27 +4173,27 @@
     </row>
     <row r="35" spans="1:27" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D35" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="E35" s="8" t="s">
         <v>137</v>
       </c>
-      <c r="E35" s="8" t="s">
+      <c r="F35" s="9" t="s">
         <v>138</v>
-      </c>
-      <c r="F35" s="9" t="s">
-        <v>139</v>
       </c>
       <c r="G35" s="9"/>
       <c r="H35" s="9"/>
       <c r="I35" s="9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J35" s="10"/>
       <c r="K35" s="10"/>
@@ -4222,27 +4216,27 @@
     </row>
     <row r="36" spans="1:27" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D36" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="E36" s="8" t="s">
         <v>140</v>
       </c>
-      <c r="E36" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="F36" s="21" t="s">
-        <v>260</v>
+      <c r="F36" s="9" t="s">
+        <v>259</v>
       </c>
       <c r="G36" s="9"/>
       <c r="H36" s="9"/>
       <c r="I36" s="9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J36" s="10"/>
       <c r="K36" s="10"/>
@@ -4265,29 +4259,29 @@
     </row>
     <row r="37" spans="1:27" ht="250.8" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C37" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="D37" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="D37" s="8" t="s">
+      <c r="E37" s="8" t="s">
         <v>143</v>
       </c>
-      <c r="E37" s="8" t="s">
+      <c r="F37" s="8" t="s">
         <v>144</v>
-      </c>
-      <c r="F37" s="19" t="s">
-        <v>145</v>
       </c>
       <c r="G37" s="8"/>
       <c r="H37" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="I37" s="9" t="s">
         <v>146</v>
-      </c>
-      <c r="I37" s="9" t="s">
-        <v>147</v>
       </c>
       <c r="J37" s="10"/>
       <c r="K37" s="10"/>
@@ -4310,27 +4304,27 @@
     </row>
     <row r="38" spans="1:27" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D38" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="E38" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="E38" s="8" t="s">
-        <v>149</v>
-      </c>
       <c r="F38" s="9" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G38" s="8"/>
       <c r="H38" s="9"/>
       <c r="I38" s="9" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J38" s="10"/>
       <c r="K38" s="10"/>
@@ -4353,27 +4347,27 @@
     </row>
     <row r="39" spans="1:27" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D39" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="E39" s="8" t="s">
         <v>150</v>
       </c>
-      <c r="E39" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="F39" s="21" t="s">
-        <v>260</v>
+      <c r="F39" s="9" t="s">
+        <v>259</v>
       </c>
       <c r="G39" s="8"/>
       <c r="H39" s="9"/>
       <c r="I39" s="9" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J39" s="10"/>
       <c r="K39" s="10"/>
@@ -4396,29 +4390,29 @@
     </row>
     <row r="40" spans="1:27" ht="211.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C40" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="D40" s="8" t="s">
         <v>152</v>
       </c>
-      <c r="D40" s="8" t="s">
+      <c r="E40" s="8" t="s">
         <v>153</v>
       </c>
-      <c r="E40" s="8" t="s">
-        <v>154</v>
-      </c>
       <c r="F40" s="8" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="G40" s="8"/>
       <c r="H40" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="I40" s="9" t="s">
         <v>155</v>
-      </c>
-      <c r="I40" s="9" t="s">
-        <v>156</v>
       </c>
       <c r="J40" s="10"/>
       <c r="K40" s="10"/>
@@ -4441,27 +4435,27 @@
     </row>
     <row r="41" spans="1:27" ht="92.4" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D41" s="8"/>
       <c r="E41" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="F41" s="8" t="s">
+        <v>250</v>
+      </c>
+      <c r="G41" s="9" t="s">
         <v>158</v>
-      </c>
-      <c r="F41" s="19" t="s">
-        <v>251</v>
-      </c>
-      <c r="G41" s="9" t="s">
-        <v>159</v>
       </c>
       <c r="H41" s="9"/>
       <c r="I41" s="9" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="J41" s="10"/>
       <c r="K41" s="10"/>
@@ -4484,27 +4478,27 @@
     </row>
     <row r="42" spans="1:27" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D42" s="8"/>
       <c r="E42" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="F42" s="8" t="s">
         <v>162</v>
       </c>
-      <c r="F42" s="8" t="s">
+      <c r="G42" s="9" t="s">
         <v>163</v>
-      </c>
-      <c r="G42" s="9" t="s">
-        <v>164</v>
       </c>
       <c r="H42" s="9"/>
       <c r="I42" s="9" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="J42" s="10"/>
       <c r="K42" s="10"/>
@@ -4527,27 +4521,27 @@
     </row>
     <row r="43" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C43" s="8" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D43" s="8"/>
       <c r="E43" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="F43" s="8" t="s">
         <v>166</v>
       </c>
-      <c r="F43" s="8" t="s">
+      <c r="G43" s="12" t="s">
         <v>167</v>
-      </c>
-      <c r="G43" s="12" t="s">
-        <v>168</v>
       </c>
       <c r="H43" s="9"/>
       <c r="I43" s="9" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="J43" s="10"/>
       <c r="K43" s="10"/>
@@ -4570,28 +4564,28 @@
     </row>
     <row r="44" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A44" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C44" s="8" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D44" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="E44" s="8" t="s">
         <v>170</v>
       </c>
-      <c r="E44" s="8" t="s">
+      <c r="F44" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G44" s="8" t="s">
         <v>171</v>
       </c>
-      <c r="F44" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="G44" s="8" t="s">
+      <c r="H44" s="9" t="s">
         <v>172</v>
-      </c>
-      <c r="H44" s="9" t="s">
-        <v>173</v>
       </c>
       <c r="I44" s="9"/>
       <c r="J44" s="10"/>
@@ -4615,24 +4609,24 @@
     </row>
     <row r="45" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A45" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C45" s="8" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D45" s="8"/>
       <c r="E45" s="8" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F45" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G45" s="11"/>
       <c r="H45" s="9" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="I45" s="9"/>
       <c r="J45" s="10"/>
@@ -4656,22 +4650,22 @@
     </row>
     <row r="46" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A46" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C46" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="D46" s="8" t="s">
         <v>177</v>
       </c>
-      <c r="D46" s="8" t="s">
+      <c r="E46" s="8" t="s">
         <v>178</v>
       </c>
-      <c r="E46" s="8" t="s">
-        <v>179</v>
-      </c>
       <c r="F46" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G46" s="8"/>
       <c r="H46" s="9"/>
@@ -4697,29 +4691,29 @@
     </row>
     <row r="47" spans="1:27" ht="105.6" x14ac:dyDescent="0.25">
       <c r="A47" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B47" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="C47" s="8" t="s">
         <v>180</v>
       </c>
-      <c r="C47" s="8" t="s">
+      <c r="D47" s="8" t="s">
         <v>181</v>
       </c>
-      <c r="D47" s="8" t="s">
+      <c r="E47" s="8" t="s">
         <v>182</v>
       </c>
-      <c r="E47" s="8" t="s">
+      <c r="F47" s="8" t="s">
         <v>183</v>
-      </c>
-      <c r="F47" s="8" t="s">
-        <v>184</v>
       </c>
       <c r="G47" s="8"/>
       <c r="H47" s="9" t="s">
+        <v>184</v>
+      </c>
+      <c r="I47" s="9" t="s">
         <v>185</v>
-      </c>
-      <c r="I47" s="9" t="s">
-        <v>186</v>
       </c>
       <c r="J47" s="10"/>
       <c r="K47" s="10"/>
@@ -4742,26 +4736,26 @@
     </row>
     <row r="48" spans="1:27" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A48" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B48" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="C48" s="8" t="s">
         <v>180</v>
       </c>
-      <c r="C48" s="8" t="s">
-        <v>181</v>
-      </c>
       <c r="D48" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="E48" s="8" t="s">
         <v>187</v>
       </c>
-      <c r="E48" s="8" t="s">
+      <c r="F48" s="11" t="s">
         <v>188</v>
-      </c>
-      <c r="F48" s="11" t="s">
-        <v>189</v>
       </c>
       <c r="G48" s="11"/>
       <c r="H48" s="9" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="I48" s="9"/>
       <c r="J48" s="10"/>
@@ -4785,29 +4779,29 @@
     </row>
     <row r="49" spans="1:27" ht="198" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B49" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="C49" s="8" t="s">
         <v>180</v>
       </c>
-      <c r="C49" s="8" t="s">
-        <v>181</v>
-      </c>
       <c r="D49" s="8" t="s">
+        <v>190</v>
+      </c>
+      <c r="E49" s="8" t="s">
         <v>191</v>
       </c>
-      <c r="E49" s="8" t="s">
+      <c r="F49" s="8" t="s">
         <v>192</v>
       </c>
-      <c r="F49" s="19" t="s">
-        <v>193</v>
-      </c>
-      <c r="G49" s="21" t="s">
-        <v>244</v>
+      <c r="G49" s="9" t="s">
+        <v>243</v>
       </c>
       <c r="H49" s="9"/>
       <c r="I49" s="9" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="J49" s="10"/>
       <c r="K49" s="10"/>
@@ -4830,29 +4824,29 @@
     </row>
     <row r="50" spans="1:27" ht="224.4" x14ac:dyDescent="0.25">
       <c r="A50" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B50" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="C50" s="8" t="s">
         <v>180</v>
       </c>
-      <c r="C50" s="8" t="s">
-        <v>181</v>
-      </c>
       <c r="D50" s="8" t="s">
+        <v>194</v>
+      </c>
+      <c r="E50" s="8" t="s">
         <v>195</v>
       </c>
-      <c r="E50" s="8" t="s">
+      <c r="F50" s="8" t="s">
         <v>196</v>
       </c>
-      <c r="F50" s="19" t="s">
-        <v>197</v>
-      </c>
-      <c r="G50" s="21" t="s">
-        <v>245</v>
+      <c r="G50" s="9" t="s">
+        <v>244</v>
       </c>
       <c r="H50" s="9"/>
       <c r="I50" s="9" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="J50" s="10"/>
       <c r="K50" s="10"/>
@@ -4875,26 +4869,26 @@
     </row>
     <row r="51" spans="1:27" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A51" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B51" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="C51" s="8" t="s">
         <v>180</v>
       </c>
-      <c r="C51" s="8" t="s">
-        <v>181</v>
-      </c>
       <c r="D51" s="8" t="s">
+        <v>197</v>
+      </c>
+      <c r="E51" s="8" t="s">
         <v>198</v>
       </c>
-      <c r="E51" s="8" t="s">
-        <v>199</v>
-      </c>
       <c r="F51" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G51" s="11"/>
       <c r="H51" s="9" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="I51" s="9"/>
       <c r="J51" s="10"/>
@@ -4918,27 +4912,27 @@
     </row>
     <row r="52" spans="1:27" ht="171.6" x14ac:dyDescent="0.25">
       <c r="A52" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B52" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="C52" s="8" t="s">
         <v>180</v>
       </c>
-      <c r="C52" s="8" t="s">
-        <v>181</v>
-      </c>
       <c r="D52" s="8" t="s">
+        <v>200</v>
+      </c>
+      <c r="E52" s="8" t="s">
         <v>201</v>
       </c>
-      <c r="E52" s="8" t="s">
+      <c r="F52" s="8" t="s">
         <v>202</v>
-      </c>
-      <c r="F52" s="19" t="s">
-        <v>203</v>
       </c>
       <c r="G52" s="8"/>
       <c r="H52" s="9"/>
       <c r="I52" s="9" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="J52" s="10"/>
       <c r="K52" s="10"/>
@@ -4961,27 +4955,27 @@
     </row>
     <row r="53" spans="1:27" ht="211.2" x14ac:dyDescent="0.25">
       <c r="A53" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B53" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="C53" s="8" t="s">
         <v>180</v>
       </c>
-      <c r="C53" s="8" t="s">
-        <v>181</v>
-      </c>
       <c r="D53" s="8" t="s">
+        <v>204</v>
+      </c>
+      <c r="E53" s="8" t="s">
         <v>205</v>
       </c>
-      <c r="E53" s="8" t="s">
+      <c r="F53" s="8" t="s">
         <v>206</v>
-      </c>
-      <c r="F53" s="19" t="s">
-        <v>207</v>
       </c>
       <c r="G53" s="8"/>
       <c r="H53" s="9"/>
       <c r="I53" s="9" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="J53" s="10"/>
       <c r="K53" s="10"/>
@@ -5004,29 +4998,29 @@
     </row>
     <row r="54" spans="1:27" ht="184.8" x14ac:dyDescent="0.25">
       <c r="A54" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B54" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="C54" s="8" t="s">
         <v>180</v>
       </c>
-      <c r="C54" s="8" t="s">
-        <v>181</v>
-      </c>
       <c r="D54" s="8" t="s">
+        <v>207</v>
+      </c>
+      <c r="E54" s="8" t="s">
         <v>208</v>
       </c>
-      <c r="E54" s="8" t="s">
+      <c r="F54" s="8" t="s">
+        <v>245</v>
+      </c>
+      <c r="G54" s="8" t="s">
         <v>209</v>
-      </c>
-      <c r="F54" s="19" t="s">
-        <v>246</v>
-      </c>
-      <c r="G54" s="8" t="s">
-        <v>210</v>
       </c>
       <c r="H54" s="9"/>
       <c r="I54" s="9" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="J54" s="10"/>
       <c r="K54" s="10"/>
@@ -5049,29 +5043,29 @@
     </row>
     <row r="55" spans="1:27" ht="356.4" x14ac:dyDescent="0.25">
       <c r="A55" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B55" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="C55" s="8" t="s">
         <v>180</v>
       </c>
-      <c r="C55" s="8" t="s">
-        <v>181</v>
-      </c>
       <c r="D55" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="E55" s="8" t="s">
         <v>212</v>
       </c>
-      <c r="E55" s="8" t="s">
+      <c r="F55" s="8" t="s">
+        <v>246</v>
+      </c>
+      <c r="G55" s="8" t="s">
         <v>213</v>
-      </c>
-      <c r="F55" s="19" t="s">
-        <v>247</v>
-      </c>
-      <c r="G55" s="8" t="s">
-        <v>214</v>
       </c>
       <c r="H55" s="9"/>
       <c r="I55" s="9" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="J55" s="10"/>
       <c r="K55" s="10"/>
@@ -5094,25 +5088,25 @@
     </row>
     <row r="56" spans="1:27" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A56" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B56" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="C56" s="8" t="s">
         <v>180</v>
       </c>
-      <c r="C56" s="8" t="s">
-        <v>181</v>
-      </c>
       <c r="D56" s="8" t="s">
+        <v>215</v>
+      </c>
+      <c r="E56" s="8" t="s">
         <v>216</v>
       </c>
-      <c r="E56" s="8" t="s">
+      <c r="F56" s="8" t="s">
         <v>217</v>
       </c>
-      <c r="F56" s="8" t="s">
+      <c r="G56" s="8" t="s">
         <v>218</v>
-      </c>
-      <c r="G56" s="8" t="s">
-        <v>219</v>
       </c>
       <c r="H56" s="9"/>
       <c r="I56" s="9"/>
@@ -5137,22 +5131,22 @@
     </row>
     <row r="57" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A57" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B57" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="C57" s="8" t="s">
         <v>180</v>
       </c>
-      <c r="C57" s="8" t="s">
-        <v>181</v>
-      </c>
       <c r="D57" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="E57" s="8" t="s">
         <v>220</v>
       </c>
-      <c r="E57" s="8" t="s">
-        <v>221</v>
-      </c>
       <c r="F57" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G57" s="11"/>
       <c r="H57" s="9"/>
@@ -5178,26 +5172,26 @@
     </row>
     <row r="58" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A58" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B58" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="C58" s="8" t="s">
         <v>180</v>
       </c>
-      <c r="C58" s="8" t="s">
-        <v>181</v>
-      </c>
       <c r="D58" s="8" t="s">
+        <v>221</v>
+      </c>
+      <c r="E58" s="8" t="s">
         <v>222</v>
       </c>
-      <c r="E58" s="8" t="s">
-        <v>223</v>
-      </c>
       <c r="F58" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G58" s="8"/>
       <c r="H58" s="9" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="I58" s="9"/>
       <c r="J58" s="10"/>
@@ -5221,22 +5215,22 @@
     </row>
     <row r="59" spans="1:27" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B59" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="C59" s="8" t="s">
         <v>180</v>
       </c>
-      <c r="C59" s="8" t="s">
-        <v>181</v>
-      </c>
       <c r="D59" s="8" t="s">
+        <v>223</v>
+      </c>
+      <c r="E59" s="8" t="s">
         <v>224</v>
       </c>
-      <c r="E59" s="8" t="s">
+      <c r="F59" s="8" t="s">
         <v>225</v>
-      </c>
-      <c r="F59" s="8" t="s">
-        <v>226</v>
       </c>
       <c r="G59" s="8"/>
       <c r="H59" s="9"/>
@@ -5262,26 +5256,26 @@
     </row>
     <row r="60" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A60" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B60" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="C60" s="8" t="s">
         <v>180</v>
       </c>
-      <c r="C60" s="8" t="s">
-        <v>181</v>
-      </c>
       <c r="D60" s="8" t="s">
+        <v>226</v>
+      </c>
+      <c r="E60" s="8" t="s">
         <v>227</v>
       </c>
-      <c r="E60" s="8" t="s">
-        <v>228</v>
-      </c>
       <c r="F60" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G60" s="11"/>
       <c r="H60" s="9" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="I60" s="9"/>
       <c r="J60" s="10"/>
@@ -5305,26 +5299,26 @@
     </row>
     <row r="61" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A61" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B61" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="C61" s="8" t="s">
         <v>180</v>
       </c>
-      <c r="C61" s="8" t="s">
-        <v>181</v>
-      </c>
       <c r="D61" s="8" t="s">
+        <v>228</v>
+      </c>
+      <c r="E61" s="8" t="s">
         <v>229</v>
       </c>
-      <c r="E61" s="8" t="s">
-        <v>230</v>
-      </c>
       <c r="F61" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G61" s="11"/>
       <c r="H61" s="9" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="I61" s="9"/>
       <c r="J61" s="10"/>
@@ -5348,22 +5342,22 @@
     </row>
     <row r="62" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A62" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B62" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="C62" s="8" t="s">
         <v>180</v>
       </c>
-      <c r="C62" s="8" t="s">
-        <v>181</v>
-      </c>
       <c r="D62" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E62" s="8" t="s">
-        <v>232</v>
-      </c>
-      <c r="F62" s="19" t="s">
-        <v>261</v>
+        <v>231</v>
+      </c>
+      <c r="F62" s="8" t="s">
+        <v>260</v>
       </c>
       <c r="G62" s="8"/>
       <c r="H62" s="9"/>
@@ -5389,31 +5383,31 @@
     </row>
     <row r="63" spans="1:27" ht="184.8" x14ac:dyDescent="0.25">
       <c r="A63" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B63" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C63" s="8" t="s">
+        <v>232</v>
+      </c>
+      <c r="D63" s="8" t="s">
         <v>233</v>
       </c>
-      <c r="D63" s="8" t="s">
+      <c r="E63" s="8" t="s">
         <v>234</v>
       </c>
-      <c r="E63" s="8" t="s">
+      <c r="F63" s="8" t="s">
+        <v>247</v>
+      </c>
+      <c r="G63" s="8" t="s">
+        <v>253</v>
+      </c>
+      <c r="H63" s="9" t="s">
+        <v>251</v>
+      </c>
+      <c r="I63" s="9" t="s">
         <v>235</v>
-      </c>
-      <c r="F63" s="19" t="s">
-        <v>248</v>
-      </c>
-      <c r="G63" s="8" t="s">
-        <v>254</v>
-      </c>
-      <c r="H63" s="9" t="s">
-        <v>252</v>
-      </c>
-      <c r="I63" s="9" t="s">
-        <v>236</v>
       </c>
       <c r="J63" s="10"/>
       <c r="K63" s="10"/>
@@ -5436,24 +5430,24 @@
     </row>
     <row r="64" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A64" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B64" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C64" s="8" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D64" s="11"/>
       <c r="E64" s="8" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F64" s="16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G64" s="11"/>
       <c r="H64" s="9" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="I64" s="9"/>
       <c r="J64" s="10"/>
@@ -5477,22 +5471,22 @@
     </row>
     <row r="65" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A65" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B65" s="8" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C65" s="8"/>
       <c r="D65" s="8"/>
       <c r="E65" s="8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F65" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G65" s="11"/>
       <c r="H65" s="9" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="I65" s="9"/>
       <c r="J65" s="10"/>
@@ -5516,20 +5510,20 @@
     </row>
     <row r="66" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A66" s="7" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B66" s="8"/>
       <c r="C66" s="8"/>
       <c r="D66" s="8"/>
       <c r="E66" s="8" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F66" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G66" s="11"/>
       <c r="H66" s="9" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="I66" s="9"/>
       <c r="J66" s="10"/>

</xml_diff>